<commit_message>
Fix variable Exposure and backtesting
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/59_Inst_Analysis_Unit_ISPRO.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/59_Inst_Analysis_Unit_ISPRO.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dati\DEV\GitRepoAAAP\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2625" yWindow="465" windowWidth="29385" windowHeight="13380" activeTab="2"/>
+    <workbookView xWindow="2625" yWindow="465" windowWidth="29385" windowHeight="13380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis_Unit" sheetId="1" r:id="rId1"/>
@@ -130,9 +130,6 @@
     <t>CustomerInfoFormula</t>
   </si>
   <si>
-    <t>EXPOSURE</t>
-  </si>
-  <si>
     <t>COUNTERPARTY_ISPRO</t>
   </si>
   <si>
@@ -1166,6 +1163,9 @@
   </si>
   <si>
     <t>COUNTERPARTY_ISPRO_IND_210</t>
+  </si>
+  <si>
+    <t>ISPRO_EXPOSURE</t>
   </si>
 </sst>
 </file>
@@ -1291,7 +1291,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="1026" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1339,7 +1345,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2050" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="2050" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1382,7 +1394,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1430,7 +1448,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1478,7 +1502,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1843,25 +1873,25 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
         <v>28</v>
       </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>30</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>31</v>
-      </c>
-      <c r="I3" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1875,8 +1905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F172"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="I166" sqref="I166"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1885,10 +1915,10 @@
     <col min="2" max="3" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -1923,16 +1953,16 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1940,16 +1970,16 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1957,16 +1987,16 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1974,16 +2004,16 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>371</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1991,16 +2021,16 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2008,16 +2038,16 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="C8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2025,16 +2055,16 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2042,16 +2072,16 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="C10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2059,16 +2089,16 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="C11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2076,16 +2106,16 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="C12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2093,16 +2123,16 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="C13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2110,16 +2140,16 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="C14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2127,16 +2157,16 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="C15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2144,16 +2174,16 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="C16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2161,16 +2191,16 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="C17" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2178,16 +2208,16 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="C18" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2195,16 +2225,16 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="C19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2212,16 +2242,16 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="C20" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2229,16 +2259,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="C21" t="s">
-        <v>68</v>
-      </c>
-      <c r="E21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2246,16 +2276,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="C22" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2263,16 +2293,16 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="C23" t="s">
-        <v>72</v>
-      </c>
-      <c r="E23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2280,16 +2310,16 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="C24" t="s">
-        <v>74</v>
-      </c>
-      <c r="E24" t="s">
-        <v>27</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2297,16 +2327,16 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="C25" t="s">
-        <v>76</v>
-      </c>
-      <c r="E25" t="s">
-        <v>27</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2314,16 +2344,16 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="C26" t="s">
-        <v>78</v>
-      </c>
-      <c r="E26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2331,16 +2361,16 @@
         <v>20</v>
       </c>
       <c r="B27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="C27" t="s">
-        <v>80</v>
-      </c>
-      <c r="E27" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2348,16 +2378,16 @@
         <v>20</v>
       </c>
       <c r="B28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="C28" t="s">
-        <v>82</v>
-      </c>
-      <c r="E28" t="s">
-        <v>27</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2365,16 +2395,16 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="C29" t="s">
-        <v>84</v>
-      </c>
-      <c r="E29" t="s">
-        <v>27</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2382,16 +2412,16 @@
         <v>20</v>
       </c>
       <c r="B30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="C30" t="s">
-        <v>86</v>
-      </c>
-      <c r="E30" t="s">
-        <v>27</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2399,16 +2429,16 @@
         <v>20</v>
       </c>
       <c r="B31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" t="s">
+        <v>87</v>
+      </c>
+      <c r="E31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="C31" t="s">
-        <v>88</v>
-      </c>
-      <c r="E31" t="s">
-        <v>27</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2416,16 +2446,16 @@
         <v>20</v>
       </c>
       <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" t="s">
+        <v>89</v>
+      </c>
+      <c r="E32" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="C32" t="s">
-        <v>90</v>
-      </c>
-      <c r="E32" t="s">
-        <v>27</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2433,16 +2463,16 @@
         <v>20</v>
       </c>
       <c r="B33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="C33" t="s">
-        <v>92</v>
-      </c>
-      <c r="E33" t="s">
-        <v>27</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2450,16 +2480,16 @@
         <v>20</v>
       </c>
       <c r="B34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" t="s">
+        <v>93</v>
+      </c>
+      <c r="E34" t="s">
+        <v>26</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="C34" t="s">
-        <v>94</v>
-      </c>
-      <c r="E34" t="s">
-        <v>27</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2467,16 +2497,16 @@
         <v>20</v>
       </c>
       <c r="B35" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" t="s">
+        <v>95</v>
+      </c>
+      <c r="E35" t="s">
+        <v>26</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="C35" t="s">
-        <v>96</v>
-      </c>
-      <c r="E35" t="s">
-        <v>27</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2484,16 +2514,16 @@
         <v>20</v>
       </c>
       <c r="B36" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" t="s">
+        <v>97</v>
+      </c>
+      <c r="E36" t="s">
+        <v>26</v>
+      </c>
+      <c r="F36" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="C36" t="s">
-        <v>98</v>
-      </c>
-      <c r="E36" t="s">
-        <v>27</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2501,16 +2531,16 @@
         <v>20</v>
       </c>
       <c r="B37" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" t="s">
+        <v>99</v>
+      </c>
+      <c r="E37" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="C37" t="s">
-        <v>100</v>
-      </c>
-      <c r="E37" t="s">
-        <v>27</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2518,16 +2548,16 @@
         <v>20</v>
       </c>
       <c r="B38" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" t="s">
+        <v>101</v>
+      </c>
+      <c r="E38" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="C38" t="s">
-        <v>102</v>
-      </c>
-      <c r="E38" t="s">
-        <v>27</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2535,16 +2565,16 @@
         <v>20</v>
       </c>
       <c r="B39" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" t="s">
+        <v>103</v>
+      </c>
+      <c r="E39" t="s">
+        <v>26</v>
+      </c>
+      <c r="F39" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="C39" t="s">
-        <v>104</v>
-      </c>
-      <c r="E39" t="s">
-        <v>27</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2552,16 +2582,16 @@
         <v>20</v>
       </c>
       <c r="B40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" t="s">
+        <v>105</v>
+      </c>
+      <c r="E40" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="C40" t="s">
-        <v>106</v>
-      </c>
-      <c r="E40" t="s">
-        <v>27</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2569,16 +2599,16 @@
         <v>20</v>
       </c>
       <c r="B41" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" t="s">
+        <v>107</v>
+      </c>
+      <c r="E41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F41" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="C41" t="s">
-        <v>108</v>
-      </c>
-      <c r="E41" t="s">
-        <v>27</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2586,16 +2616,16 @@
         <v>20</v>
       </c>
       <c r="B42" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" t="s">
+        <v>109</v>
+      </c>
+      <c r="E42" t="s">
+        <v>26</v>
+      </c>
+      <c r="F42" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="C42" t="s">
-        <v>110</v>
-      </c>
-      <c r="E42" t="s">
-        <v>27</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2603,16 +2633,16 @@
         <v>20</v>
       </c>
       <c r="B43" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" t="s">
+        <v>111</v>
+      </c>
+      <c r="E43" t="s">
+        <v>26</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="C43" t="s">
-        <v>112</v>
-      </c>
-      <c r="E43" t="s">
-        <v>27</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2620,16 +2650,16 @@
         <v>20</v>
       </c>
       <c r="B44" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" t="s">
+        <v>113</v>
+      </c>
+      <c r="E44" t="s">
+        <v>26</v>
+      </c>
+      <c r="F44" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="C44" t="s">
-        <v>114</v>
-      </c>
-      <c r="E44" t="s">
-        <v>27</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2637,16 +2667,16 @@
         <v>20</v>
       </c>
       <c r="B45" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45" t="s">
+        <v>115</v>
+      </c>
+      <c r="E45" t="s">
+        <v>26</v>
+      </c>
+      <c r="F45" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="C45" t="s">
-        <v>116</v>
-      </c>
-      <c r="E45" t="s">
-        <v>27</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2654,16 +2684,16 @@
         <v>20</v>
       </c>
       <c r="B46" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46" t="s">
+        <v>117</v>
+      </c>
+      <c r="E46" t="s">
+        <v>26</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="C46" t="s">
-        <v>118</v>
-      </c>
-      <c r="E46" t="s">
-        <v>27</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2671,16 +2701,16 @@
         <v>20</v>
       </c>
       <c r="B47" t="s">
+        <v>119</v>
+      </c>
+      <c r="C47" t="s">
+        <v>119</v>
+      </c>
+      <c r="E47" t="s">
+        <v>26</v>
+      </c>
+      <c r="F47" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="C47" t="s">
-        <v>120</v>
-      </c>
-      <c r="E47" t="s">
-        <v>27</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2688,16 +2718,16 @@
         <v>20</v>
       </c>
       <c r="B48" t="s">
+        <v>121</v>
+      </c>
+      <c r="C48" t="s">
+        <v>121</v>
+      </c>
+      <c r="E48" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="C48" t="s">
-        <v>122</v>
-      </c>
-      <c r="E48" t="s">
-        <v>27</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2705,16 +2735,16 @@
         <v>20</v>
       </c>
       <c r="B49" t="s">
+        <v>123</v>
+      </c>
+      <c r="C49" t="s">
+        <v>123</v>
+      </c>
+      <c r="E49" t="s">
+        <v>26</v>
+      </c>
+      <c r="F49" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="C49" t="s">
-        <v>124</v>
-      </c>
-      <c r="E49" t="s">
-        <v>27</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2722,16 +2752,16 @@
         <v>20</v>
       </c>
       <c r="B50" t="s">
+        <v>125</v>
+      </c>
+      <c r="C50" t="s">
+        <v>125</v>
+      </c>
+      <c r="E50" t="s">
+        <v>26</v>
+      </c>
+      <c r="F50" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="C50" t="s">
-        <v>126</v>
-      </c>
-      <c r="E50" t="s">
-        <v>27</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2739,16 +2769,16 @@
         <v>20</v>
       </c>
       <c r="B51" t="s">
+        <v>127</v>
+      </c>
+      <c r="C51" t="s">
+        <v>127</v>
+      </c>
+      <c r="E51" t="s">
+        <v>26</v>
+      </c>
+      <c r="F51" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="C51" t="s">
-        <v>128</v>
-      </c>
-      <c r="E51" t="s">
-        <v>27</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2756,16 +2786,16 @@
         <v>20</v>
       </c>
       <c r="B52" t="s">
+        <v>129</v>
+      </c>
+      <c r="C52" t="s">
+        <v>129</v>
+      </c>
+      <c r="E52" t="s">
+        <v>26</v>
+      </c>
+      <c r="F52" s="5" t="s">
         <v>130</v>
-      </c>
-      <c r="C52" t="s">
-        <v>130</v>
-      </c>
-      <c r="E52" t="s">
-        <v>27</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2773,16 +2803,16 @@
         <v>20</v>
       </c>
       <c r="B53" t="s">
+        <v>131</v>
+      </c>
+      <c r="C53" t="s">
+        <v>131</v>
+      </c>
+      <c r="E53" t="s">
+        <v>26</v>
+      </c>
+      <c r="F53" s="5" t="s">
         <v>132</v>
-      </c>
-      <c r="C53" t="s">
-        <v>132</v>
-      </c>
-      <c r="E53" t="s">
-        <v>27</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2790,16 +2820,16 @@
         <v>20</v>
       </c>
       <c r="B54" t="s">
+        <v>133</v>
+      </c>
+      <c r="C54" t="s">
+        <v>133</v>
+      </c>
+      <c r="E54" t="s">
+        <v>26</v>
+      </c>
+      <c r="F54" s="5" t="s">
         <v>134</v>
-      </c>
-      <c r="C54" t="s">
-        <v>134</v>
-      </c>
-      <c r="E54" t="s">
-        <v>27</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2807,16 +2837,16 @@
         <v>20</v>
       </c>
       <c r="B55" t="s">
+        <v>135</v>
+      </c>
+      <c r="C55" t="s">
+        <v>135</v>
+      </c>
+      <c r="E55" t="s">
+        <v>26</v>
+      </c>
+      <c r="F55" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="C55" t="s">
-        <v>136</v>
-      </c>
-      <c r="E55" t="s">
-        <v>27</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2824,16 +2854,16 @@
         <v>20</v>
       </c>
       <c r="B56" t="s">
+        <v>137</v>
+      </c>
+      <c r="C56" t="s">
+        <v>137</v>
+      </c>
+      <c r="E56" t="s">
+        <v>26</v>
+      </c>
+      <c r="F56" s="5" t="s">
         <v>138</v>
-      </c>
-      <c r="C56" t="s">
-        <v>138</v>
-      </c>
-      <c r="E56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2841,16 +2871,16 @@
         <v>20</v>
       </c>
       <c r="B57" t="s">
+        <v>139</v>
+      </c>
+      <c r="C57" t="s">
+        <v>139</v>
+      </c>
+      <c r="E57" t="s">
+        <v>26</v>
+      </c>
+      <c r="F57" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="C57" t="s">
-        <v>140</v>
-      </c>
-      <c r="E57" t="s">
-        <v>27</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2858,16 +2888,16 @@
         <v>20</v>
       </c>
       <c r="B58" t="s">
+        <v>141</v>
+      </c>
+      <c r="C58" t="s">
+        <v>141</v>
+      </c>
+      <c r="E58" t="s">
+        <v>26</v>
+      </c>
+      <c r="F58" s="5" t="s">
         <v>142</v>
-      </c>
-      <c r="C58" t="s">
-        <v>142</v>
-      </c>
-      <c r="E58" t="s">
-        <v>27</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2875,16 +2905,16 @@
         <v>20</v>
       </c>
       <c r="B59" t="s">
+        <v>143</v>
+      </c>
+      <c r="C59" t="s">
+        <v>143</v>
+      </c>
+      <c r="E59" t="s">
+        <v>26</v>
+      </c>
+      <c r="F59" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="C59" t="s">
-        <v>144</v>
-      </c>
-      <c r="E59" t="s">
-        <v>27</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2892,16 +2922,16 @@
         <v>20</v>
       </c>
       <c r="B60" t="s">
+        <v>145</v>
+      </c>
+      <c r="C60" t="s">
+        <v>145</v>
+      </c>
+      <c r="E60" t="s">
+        <v>26</v>
+      </c>
+      <c r="F60" s="5" t="s">
         <v>146</v>
-      </c>
-      <c r="C60" t="s">
-        <v>146</v>
-      </c>
-      <c r="E60" t="s">
-        <v>27</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2909,16 +2939,16 @@
         <v>20</v>
       </c>
       <c r="B61" t="s">
+        <v>147</v>
+      </c>
+      <c r="C61" t="s">
+        <v>147</v>
+      </c>
+      <c r="E61" t="s">
+        <v>26</v>
+      </c>
+      <c r="F61" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="C61" t="s">
-        <v>148</v>
-      </c>
-      <c r="E61" t="s">
-        <v>27</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2926,16 +2956,16 @@
         <v>20</v>
       </c>
       <c r="B62" t="s">
+        <v>149</v>
+      </c>
+      <c r="C62" t="s">
+        <v>149</v>
+      </c>
+      <c r="E62" t="s">
+        <v>26</v>
+      </c>
+      <c r="F62" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="C62" t="s">
-        <v>150</v>
-      </c>
-      <c r="E62" t="s">
-        <v>27</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2943,16 +2973,16 @@
         <v>20</v>
       </c>
       <c r="B63" t="s">
+        <v>151</v>
+      </c>
+      <c r="C63" t="s">
+        <v>151</v>
+      </c>
+      <c r="E63" t="s">
+        <v>26</v>
+      </c>
+      <c r="F63" s="5" t="s">
         <v>152</v>
-      </c>
-      <c r="C63" t="s">
-        <v>152</v>
-      </c>
-      <c r="E63" t="s">
-        <v>27</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2960,16 +2990,16 @@
         <v>20</v>
       </c>
       <c r="B64" t="s">
+        <v>153</v>
+      </c>
+      <c r="C64" t="s">
+        <v>153</v>
+      </c>
+      <c r="E64" t="s">
+        <v>26</v>
+      </c>
+      <c r="F64" s="5" t="s">
         <v>154</v>
-      </c>
-      <c r="C64" t="s">
-        <v>154</v>
-      </c>
-      <c r="E64" t="s">
-        <v>27</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2977,16 +3007,16 @@
         <v>20</v>
       </c>
       <c r="B65" t="s">
+        <v>155</v>
+      </c>
+      <c r="C65" t="s">
+        <v>155</v>
+      </c>
+      <c r="E65" t="s">
+        <v>26</v>
+      </c>
+      <c r="F65" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="C65" t="s">
-        <v>156</v>
-      </c>
-      <c r="E65" t="s">
-        <v>27</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2994,16 +3024,16 @@
         <v>20</v>
       </c>
       <c r="B66" t="s">
+        <v>157</v>
+      </c>
+      <c r="C66" t="s">
+        <v>157</v>
+      </c>
+      <c r="E66" t="s">
+        <v>26</v>
+      </c>
+      <c r="F66" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="C66" t="s">
-        <v>158</v>
-      </c>
-      <c r="E66" t="s">
-        <v>27</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -3011,16 +3041,16 @@
         <v>20</v>
       </c>
       <c r="B67" t="s">
+        <v>159</v>
+      </c>
+      <c r="C67" t="s">
+        <v>159</v>
+      </c>
+      <c r="E67" t="s">
+        <v>26</v>
+      </c>
+      <c r="F67" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="C67" t="s">
-        <v>160</v>
-      </c>
-      <c r="E67" t="s">
-        <v>27</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -3028,16 +3058,16 @@
         <v>20</v>
       </c>
       <c r="B68" t="s">
+        <v>161</v>
+      </c>
+      <c r="C68" t="s">
+        <v>161</v>
+      </c>
+      <c r="E68" t="s">
+        <v>26</v>
+      </c>
+      <c r="F68" s="5" t="s">
         <v>162</v>
-      </c>
-      <c r="C68" t="s">
-        <v>162</v>
-      </c>
-      <c r="E68" t="s">
-        <v>27</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -3045,16 +3075,16 @@
         <v>20</v>
       </c>
       <c r="B69" t="s">
+        <v>163</v>
+      </c>
+      <c r="C69" t="s">
+        <v>163</v>
+      </c>
+      <c r="E69" t="s">
+        <v>26</v>
+      </c>
+      <c r="F69" s="5" t="s">
         <v>164</v>
-      </c>
-      <c r="C69" t="s">
-        <v>164</v>
-      </c>
-      <c r="E69" t="s">
-        <v>27</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -3062,16 +3092,16 @@
         <v>20</v>
       </c>
       <c r="B70" t="s">
+        <v>165</v>
+      </c>
+      <c r="C70" t="s">
+        <v>165</v>
+      </c>
+      <c r="E70" t="s">
+        <v>26</v>
+      </c>
+      <c r="F70" s="5" t="s">
         <v>166</v>
-      </c>
-      <c r="C70" t="s">
-        <v>166</v>
-      </c>
-      <c r="E70" t="s">
-        <v>27</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -3079,16 +3109,16 @@
         <v>20</v>
       </c>
       <c r="B71" t="s">
+        <v>167</v>
+      </c>
+      <c r="C71" t="s">
+        <v>167</v>
+      </c>
+      <c r="E71" t="s">
+        <v>26</v>
+      </c>
+      <c r="F71" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="C71" t="s">
-        <v>168</v>
-      </c>
-      <c r="E71" t="s">
-        <v>27</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -3096,16 +3126,16 @@
         <v>20</v>
       </c>
       <c r="B72" t="s">
+        <v>169</v>
+      </c>
+      <c r="C72" t="s">
+        <v>169</v>
+      </c>
+      <c r="E72" t="s">
+        <v>26</v>
+      </c>
+      <c r="F72" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="C72" t="s">
-        <v>170</v>
-      </c>
-      <c r="E72" t="s">
-        <v>27</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -3113,16 +3143,16 @@
         <v>20</v>
       </c>
       <c r="B73" t="s">
+        <v>171</v>
+      </c>
+      <c r="C73" t="s">
+        <v>171</v>
+      </c>
+      <c r="E73" t="s">
+        <v>26</v>
+      </c>
+      <c r="F73" s="5" t="s">
         <v>172</v>
-      </c>
-      <c r="C73" t="s">
-        <v>172</v>
-      </c>
-      <c r="E73" t="s">
-        <v>27</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -3130,16 +3160,16 @@
         <v>20</v>
       </c>
       <c r="B74" t="s">
+        <v>173</v>
+      </c>
+      <c r="C74" t="s">
+        <v>173</v>
+      </c>
+      <c r="E74" t="s">
+        <v>26</v>
+      </c>
+      <c r="F74" s="5" t="s">
         <v>174</v>
-      </c>
-      <c r="C74" t="s">
-        <v>174</v>
-      </c>
-      <c r="E74" t="s">
-        <v>27</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -3147,16 +3177,16 @@
         <v>20</v>
       </c>
       <c r="B75" t="s">
+        <v>175</v>
+      </c>
+      <c r="C75" t="s">
+        <v>175</v>
+      </c>
+      <c r="E75" t="s">
+        <v>26</v>
+      </c>
+      <c r="F75" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="C75" t="s">
-        <v>176</v>
-      </c>
-      <c r="E75" t="s">
-        <v>27</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -3164,16 +3194,16 @@
         <v>20</v>
       </c>
       <c r="B76" t="s">
+        <v>177</v>
+      </c>
+      <c r="C76" t="s">
+        <v>177</v>
+      </c>
+      <c r="E76" t="s">
+        <v>26</v>
+      </c>
+      <c r="F76" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="C76" t="s">
-        <v>178</v>
-      </c>
-      <c r="E76" t="s">
-        <v>27</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -3181,16 +3211,16 @@
         <v>20</v>
       </c>
       <c r="B77" t="s">
+        <v>179</v>
+      </c>
+      <c r="C77" t="s">
+        <v>179</v>
+      </c>
+      <c r="E77" t="s">
+        <v>26</v>
+      </c>
+      <c r="F77" s="5" t="s">
         <v>180</v>
-      </c>
-      <c r="C77" t="s">
-        <v>180</v>
-      </c>
-      <c r="E77" t="s">
-        <v>27</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -3198,16 +3228,16 @@
         <v>20</v>
       </c>
       <c r="B78" t="s">
+        <v>181</v>
+      </c>
+      <c r="C78" t="s">
+        <v>181</v>
+      </c>
+      <c r="E78" t="s">
+        <v>26</v>
+      </c>
+      <c r="F78" s="5" t="s">
         <v>182</v>
-      </c>
-      <c r="C78" t="s">
-        <v>182</v>
-      </c>
-      <c r="E78" t="s">
-        <v>27</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -3215,16 +3245,16 @@
         <v>20</v>
       </c>
       <c r="B79" t="s">
+        <v>183</v>
+      </c>
+      <c r="C79" t="s">
+        <v>183</v>
+      </c>
+      <c r="E79" t="s">
+        <v>26</v>
+      </c>
+      <c r="F79" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="C79" t="s">
-        <v>184</v>
-      </c>
-      <c r="E79" t="s">
-        <v>27</v>
-      </c>
-      <c r="F79" s="5" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -3232,16 +3262,16 @@
         <v>20</v>
       </c>
       <c r="B80" t="s">
+        <v>185</v>
+      </c>
+      <c r="C80" t="s">
+        <v>185</v>
+      </c>
+      <c r="E80" t="s">
+        <v>26</v>
+      </c>
+      <c r="F80" s="5" t="s">
         <v>186</v>
-      </c>
-      <c r="C80" t="s">
-        <v>186</v>
-      </c>
-      <c r="E80" t="s">
-        <v>27</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -3249,16 +3279,16 @@
         <v>20</v>
       </c>
       <c r="B81" t="s">
+        <v>187</v>
+      </c>
+      <c r="C81" t="s">
+        <v>187</v>
+      </c>
+      <c r="E81" t="s">
+        <v>26</v>
+      </c>
+      <c r="F81" s="5" t="s">
         <v>188</v>
-      </c>
-      <c r="C81" t="s">
-        <v>188</v>
-      </c>
-      <c r="E81" t="s">
-        <v>27</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -3266,16 +3296,16 @@
         <v>20</v>
       </c>
       <c r="B82" t="s">
+        <v>189</v>
+      </c>
+      <c r="C82" t="s">
+        <v>189</v>
+      </c>
+      <c r="E82" t="s">
+        <v>26</v>
+      </c>
+      <c r="F82" s="5" t="s">
         <v>190</v>
-      </c>
-      <c r="C82" t="s">
-        <v>190</v>
-      </c>
-      <c r="E82" t="s">
-        <v>27</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -3283,16 +3313,16 @@
         <v>20</v>
       </c>
       <c r="B83" t="s">
+        <v>191</v>
+      </c>
+      <c r="C83" t="s">
+        <v>191</v>
+      </c>
+      <c r="E83" t="s">
+        <v>26</v>
+      </c>
+      <c r="F83" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="C83" t="s">
-        <v>192</v>
-      </c>
-      <c r="E83" t="s">
-        <v>27</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -3300,16 +3330,16 @@
         <v>20</v>
       </c>
       <c r="B84" t="s">
+        <v>193</v>
+      </c>
+      <c r="C84" t="s">
+        <v>193</v>
+      </c>
+      <c r="E84" t="s">
+        <v>26</v>
+      </c>
+      <c r="F84" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="C84" t="s">
-        <v>194</v>
-      </c>
-      <c r="E84" t="s">
-        <v>27</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -3317,16 +3347,16 @@
         <v>20</v>
       </c>
       <c r="B85" t="s">
+        <v>195</v>
+      </c>
+      <c r="C85" t="s">
+        <v>195</v>
+      </c>
+      <c r="E85" t="s">
+        <v>26</v>
+      </c>
+      <c r="F85" s="5" t="s">
         <v>196</v>
-      </c>
-      <c r="C85" t="s">
-        <v>196</v>
-      </c>
-      <c r="E85" t="s">
-        <v>27</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -3334,16 +3364,16 @@
         <v>20</v>
       </c>
       <c r="B86" t="s">
+        <v>197</v>
+      </c>
+      <c r="C86" t="s">
+        <v>197</v>
+      </c>
+      <c r="E86" t="s">
+        <v>26</v>
+      </c>
+      <c r="F86" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="C86" t="s">
-        <v>198</v>
-      </c>
-      <c r="E86" t="s">
-        <v>27</v>
-      </c>
-      <c r="F86" s="5" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -3351,16 +3381,16 @@
         <v>20</v>
       </c>
       <c r="B87" t="s">
+        <v>199</v>
+      </c>
+      <c r="C87" t="s">
+        <v>199</v>
+      </c>
+      <c r="E87" t="s">
+        <v>26</v>
+      </c>
+      <c r="F87" s="5" t="s">
         <v>200</v>
-      </c>
-      <c r="C87" t="s">
-        <v>200</v>
-      </c>
-      <c r="E87" t="s">
-        <v>27</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -3368,16 +3398,16 @@
         <v>20</v>
       </c>
       <c r="B88" t="s">
+        <v>201</v>
+      </c>
+      <c r="C88" t="s">
+        <v>201</v>
+      </c>
+      <c r="E88" t="s">
+        <v>26</v>
+      </c>
+      <c r="F88" s="5" t="s">
         <v>202</v>
-      </c>
-      <c r="C88" t="s">
-        <v>202</v>
-      </c>
-      <c r="E88" t="s">
-        <v>27</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -3385,16 +3415,16 @@
         <v>20</v>
       </c>
       <c r="B89" t="s">
+        <v>203</v>
+      </c>
+      <c r="C89" t="s">
+        <v>203</v>
+      </c>
+      <c r="E89" t="s">
+        <v>26</v>
+      </c>
+      <c r="F89" s="5" t="s">
         <v>204</v>
-      </c>
-      <c r="C89" t="s">
-        <v>204</v>
-      </c>
-      <c r="E89" t="s">
-        <v>27</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -3402,16 +3432,16 @@
         <v>20</v>
       </c>
       <c r="B90" t="s">
+        <v>205</v>
+      </c>
+      <c r="C90" t="s">
+        <v>205</v>
+      </c>
+      <c r="E90" t="s">
+        <v>26</v>
+      </c>
+      <c r="F90" s="5" t="s">
         <v>206</v>
-      </c>
-      <c r="C90" t="s">
-        <v>206</v>
-      </c>
-      <c r="E90" t="s">
-        <v>27</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -3419,16 +3449,16 @@
         <v>20</v>
       </c>
       <c r="B91" t="s">
+        <v>207</v>
+      </c>
+      <c r="C91" t="s">
+        <v>207</v>
+      </c>
+      <c r="E91" t="s">
+        <v>26</v>
+      </c>
+      <c r="F91" s="5" t="s">
         <v>208</v>
-      </c>
-      <c r="C91" t="s">
-        <v>208</v>
-      </c>
-      <c r="E91" t="s">
-        <v>27</v>
-      </c>
-      <c r="F91" s="5" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -3436,16 +3466,16 @@
         <v>20</v>
       </c>
       <c r="B92" t="s">
+        <v>209</v>
+      </c>
+      <c r="C92" t="s">
+        <v>209</v>
+      </c>
+      <c r="E92" t="s">
+        <v>26</v>
+      </c>
+      <c r="F92" s="5" t="s">
         <v>210</v>
-      </c>
-      <c r="C92" t="s">
-        <v>210</v>
-      </c>
-      <c r="E92" t="s">
-        <v>27</v>
-      </c>
-      <c r="F92" s="5" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -3453,16 +3483,16 @@
         <v>20</v>
       </c>
       <c r="B93" t="s">
+        <v>211</v>
+      </c>
+      <c r="C93" t="s">
+        <v>211</v>
+      </c>
+      <c r="E93" t="s">
+        <v>26</v>
+      </c>
+      <c r="F93" s="5" t="s">
         <v>212</v>
-      </c>
-      <c r="C93" t="s">
-        <v>212</v>
-      </c>
-      <c r="E93" t="s">
-        <v>27</v>
-      </c>
-      <c r="F93" s="5" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -3470,16 +3500,16 @@
         <v>20</v>
       </c>
       <c r="B94" t="s">
+        <v>213</v>
+      </c>
+      <c r="C94" t="s">
+        <v>213</v>
+      </c>
+      <c r="E94" t="s">
+        <v>26</v>
+      </c>
+      <c r="F94" s="5" t="s">
         <v>214</v>
-      </c>
-      <c r="C94" t="s">
-        <v>214</v>
-      </c>
-      <c r="E94" t="s">
-        <v>27</v>
-      </c>
-      <c r="F94" s="5" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -3487,16 +3517,16 @@
         <v>20</v>
       </c>
       <c r="B95" t="s">
+        <v>215</v>
+      </c>
+      <c r="C95" t="s">
+        <v>215</v>
+      </c>
+      <c r="E95" t="s">
+        <v>26</v>
+      </c>
+      <c r="F95" s="5" t="s">
         <v>216</v>
-      </c>
-      <c r="C95" t="s">
-        <v>216</v>
-      </c>
-      <c r="E95" t="s">
-        <v>27</v>
-      </c>
-      <c r="F95" s="5" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -3504,16 +3534,16 @@
         <v>20</v>
       </c>
       <c r="B96" t="s">
+        <v>217</v>
+      </c>
+      <c r="C96" t="s">
+        <v>217</v>
+      </c>
+      <c r="E96" t="s">
+        <v>26</v>
+      </c>
+      <c r="F96" s="5" t="s">
         <v>218</v>
-      </c>
-      <c r="C96" t="s">
-        <v>218</v>
-      </c>
-      <c r="E96" t="s">
-        <v>27</v>
-      </c>
-      <c r="F96" s="5" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -3521,16 +3551,16 @@
         <v>20</v>
       </c>
       <c r="B97" t="s">
+        <v>219</v>
+      </c>
+      <c r="C97" t="s">
+        <v>219</v>
+      </c>
+      <c r="E97" t="s">
+        <v>26</v>
+      </c>
+      <c r="F97" s="5" t="s">
         <v>220</v>
-      </c>
-      <c r="C97" t="s">
-        <v>220</v>
-      </c>
-      <c r="E97" t="s">
-        <v>27</v>
-      </c>
-      <c r="F97" s="5" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -3538,16 +3568,16 @@
         <v>20</v>
       </c>
       <c r="B98" t="s">
+        <v>221</v>
+      </c>
+      <c r="C98" t="s">
+        <v>221</v>
+      </c>
+      <c r="E98" t="s">
+        <v>26</v>
+      </c>
+      <c r="F98" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="C98" t="s">
-        <v>222</v>
-      </c>
-      <c r="E98" t="s">
-        <v>27</v>
-      </c>
-      <c r="F98" s="5" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -3555,16 +3585,16 @@
         <v>20</v>
       </c>
       <c r="B99" t="s">
+        <v>223</v>
+      </c>
+      <c r="C99" t="s">
+        <v>223</v>
+      </c>
+      <c r="E99" t="s">
+        <v>26</v>
+      </c>
+      <c r="F99" s="5" t="s">
         <v>224</v>
-      </c>
-      <c r="C99" t="s">
-        <v>224</v>
-      </c>
-      <c r="E99" t="s">
-        <v>27</v>
-      </c>
-      <c r="F99" s="5" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -3572,16 +3602,16 @@
         <v>20</v>
       </c>
       <c r="B100" t="s">
+        <v>225</v>
+      </c>
+      <c r="C100" t="s">
+        <v>225</v>
+      </c>
+      <c r="E100" t="s">
+        <v>26</v>
+      </c>
+      <c r="F100" s="5" t="s">
         <v>226</v>
-      </c>
-      <c r="C100" t="s">
-        <v>226</v>
-      </c>
-      <c r="E100" t="s">
-        <v>27</v>
-      </c>
-      <c r="F100" s="5" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -3589,16 +3619,16 @@
         <v>20</v>
       </c>
       <c r="B101" t="s">
+        <v>227</v>
+      </c>
+      <c r="C101" t="s">
+        <v>227</v>
+      </c>
+      <c r="E101" t="s">
+        <v>26</v>
+      </c>
+      <c r="F101" s="5" t="s">
         <v>228</v>
-      </c>
-      <c r="C101" t="s">
-        <v>228</v>
-      </c>
-      <c r="E101" t="s">
-        <v>27</v>
-      </c>
-      <c r="F101" s="5" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -3606,16 +3636,16 @@
         <v>20</v>
       </c>
       <c r="B102" t="s">
+        <v>229</v>
+      </c>
+      <c r="C102" t="s">
+        <v>229</v>
+      </c>
+      <c r="E102" t="s">
+        <v>26</v>
+      </c>
+      <c r="F102" s="5" t="s">
         <v>230</v>
-      </c>
-      <c r="C102" t="s">
-        <v>230</v>
-      </c>
-      <c r="E102" t="s">
-        <v>27</v>
-      </c>
-      <c r="F102" s="5" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -3623,16 +3653,16 @@
         <v>20</v>
       </c>
       <c r="B103" t="s">
+        <v>231</v>
+      </c>
+      <c r="C103" t="s">
+        <v>231</v>
+      </c>
+      <c r="E103" t="s">
+        <v>26</v>
+      </c>
+      <c r="F103" s="5" t="s">
         <v>232</v>
-      </c>
-      <c r="C103" t="s">
-        <v>232</v>
-      </c>
-      <c r="E103" t="s">
-        <v>27</v>
-      </c>
-      <c r="F103" s="5" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -3640,16 +3670,16 @@
         <v>20</v>
       </c>
       <c r="B104" t="s">
+        <v>233</v>
+      </c>
+      <c r="C104" t="s">
+        <v>233</v>
+      </c>
+      <c r="E104" t="s">
+        <v>26</v>
+      </c>
+      <c r="F104" s="5" t="s">
         <v>234</v>
-      </c>
-      <c r="C104" t="s">
-        <v>234</v>
-      </c>
-      <c r="E104" t="s">
-        <v>27</v>
-      </c>
-      <c r="F104" s="5" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -3657,16 +3687,16 @@
         <v>20</v>
       </c>
       <c r="B105" t="s">
+        <v>235</v>
+      </c>
+      <c r="C105" t="s">
+        <v>235</v>
+      </c>
+      <c r="E105" t="s">
+        <v>26</v>
+      </c>
+      <c r="F105" s="5" t="s">
         <v>236</v>
-      </c>
-      <c r="C105" t="s">
-        <v>236</v>
-      </c>
-      <c r="E105" t="s">
-        <v>27</v>
-      </c>
-      <c r="F105" s="5" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -3674,16 +3704,16 @@
         <v>20</v>
       </c>
       <c r="B106" t="s">
+        <v>237</v>
+      </c>
+      <c r="C106" t="s">
+        <v>237</v>
+      </c>
+      <c r="E106" t="s">
+        <v>26</v>
+      </c>
+      <c r="F106" s="5" t="s">
         <v>238</v>
-      </c>
-      <c r="C106" t="s">
-        <v>238</v>
-      </c>
-      <c r="E106" t="s">
-        <v>27</v>
-      </c>
-      <c r="F106" s="5" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -3691,16 +3721,16 @@
         <v>20</v>
       </c>
       <c r="B107" t="s">
+        <v>239</v>
+      </c>
+      <c r="C107" t="s">
+        <v>239</v>
+      </c>
+      <c r="E107" t="s">
+        <v>26</v>
+      </c>
+      <c r="F107" s="5" t="s">
         <v>240</v>
-      </c>
-      <c r="C107" t="s">
-        <v>240</v>
-      </c>
-      <c r="E107" t="s">
-        <v>27</v>
-      </c>
-      <c r="F107" s="5" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -3708,16 +3738,16 @@
         <v>20</v>
       </c>
       <c r="B108" t="s">
+        <v>241</v>
+      </c>
+      <c r="C108" t="s">
+        <v>241</v>
+      </c>
+      <c r="E108" t="s">
+        <v>26</v>
+      </c>
+      <c r="F108" s="5" t="s">
         <v>242</v>
-      </c>
-      <c r="C108" t="s">
-        <v>242</v>
-      </c>
-      <c r="E108" t="s">
-        <v>27</v>
-      </c>
-      <c r="F108" s="5" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -3725,16 +3755,16 @@
         <v>20</v>
       </c>
       <c r="B109" t="s">
+        <v>243</v>
+      </c>
+      <c r="C109" t="s">
+        <v>243</v>
+      </c>
+      <c r="E109" t="s">
+        <v>26</v>
+      </c>
+      <c r="F109" s="5" t="s">
         <v>244</v>
-      </c>
-      <c r="C109" t="s">
-        <v>244</v>
-      </c>
-      <c r="E109" t="s">
-        <v>27</v>
-      </c>
-      <c r="F109" s="5" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -3742,16 +3772,16 @@
         <v>20</v>
       </c>
       <c r="B110" t="s">
+        <v>245</v>
+      </c>
+      <c r="C110" t="s">
+        <v>245</v>
+      </c>
+      <c r="E110" t="s">
+        <v>26</v>
+      </c>
+      <c r="F110" s="5" t="s">
         <v>246</v>
-      </c>
-      <c r="C110" t="s">
-        <v>246</v>
-      </c>
-      <c r="E110" t="s">
-        <v>27</v>
-      </c>
-      <c r="F110" s="5" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -3759,16 +3789,16 @@
         <v>20</v>
       </c>
       <c r="B111" t="s">
+        <v>247</v>
+      </c>
+      <c r="C111" t="s">
+        <v>247</v>
+      </c>
+      <c r="E111" t="s">
+        <v>26</v>
+      </c>
+      <c r="F111" s="5" t="s">
         <v>248</v>
-      </c>
-      <c r="C111" t="s">
-        <v>248</v>
-      </c>
-      <c r="E111" t="s">
-        <v>27</v>
-      </c>
-      <c r="F111" s="5" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -3776,16 +3806,16 @@
         <v>20</v>
       </c>
       <c r="B112" t="s">
+        <v>249</v>
+      </c>
+      <c r="C112" t="s">
+        <v>249</v>
+      </c>
+      <c r="E112" t="s">
+        <v>26</v>
+      </c>
+      <c r="F112" s="5" t="s">
         <v>250</v>
-      </c>
-      <c r="C112" t="s">
-        <v>250</v>
-      </c>
-      <c r="E112" t="s">
-        <v>27</v>
-      </c>
-      <c r="F112" s="5" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -3793,16 +3823,16 @@
         <v>20</v>
       </c>
       <c r="B113" t="s">
+        <v>251</v>
+      </c>
+      <c r="C113" t="s">
+        <v>251</v>
+      </c>
+      <c r="E113" t="s">
+        <v>26</v>
+      </c>
+      <c r="F113" s="5" t="s">
         <v>252</v>
-      </c>
-      <c r="C113" t="s">
-        <v>252</v>
-      </c>
-      <c r="E113" t="s">
-        <v>27</v>
-      </c>
-      <c r="F113" s="5" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -3810,16 +3840,16 @@
         <v>20</v>
       </c>
       <c r="B114" t="s">
+        <v>253</v>
+      </c>
+      <c r="C114" t="s">
+        <v>253</v>
+      </c>
+      <c r="E114" t="s">
+        <v>26</v>
+      </c>
+      <c r="F114" s="5" t="s">
         <v>254</v>
-      </c>
-      <c r="C114" t="s">
-        <v>254</v>
-      </c>
-      <c r="E114" t="s">
-        <v>27</v>
-      </c>
-      <c r="F114" s="5" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3827,16 +3857,16 @@
         <v>20</v>
       </c>
       <c r="B115" t="s">
+        <v>255</v>
+      </c>
+      <c r="C115" t="s">
+        <v>255</v>
+      </c>
+      <c r="E115" t="s">
+        <v>26</v>
+      </c>
+      <c r="F115" s="5" t="s">
         <v>256</v>
-      </c>
-      <c r="C115" t="s">
-        <v>256</v>
-      </c>
-      <c r="E115" t="s">
-        <v>27</v>
-      </c>
-      <c r="F115" s="5" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3844,16 +3874,16 @@
         <v>20</v>
       </c>
       <c r="B116" t="s">
+        <v>257</v>
+      </c>
+      <c r="C116" t="s">
+        <v>257</v>
+      </c>
+      <c r="E116" t="s">
+        <v>26</v>
+      </c>
+      <c r="F116" s="5" t="s">
         <v>258</v>
-      </c>
-      <c r="C116" t="s">
-        <v>258</v>
-      </c>
-      <c r="E116" t="s">
-        <v>27</v>
-      </c>
-      <c r="F116" s="5" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -3861,16 +3891,16 @@
         <v>20</v>
       </c>
       <c r="B117" t="s">
+        <v>259</v>
+      </c>
+      <c r="C117" t="s">
+        <v>259</v>
+      </c>
+      <c r="E117" t="s">
+        <v>26</v>
+      </c>
+      <c r="F117" s="5" t="s">
         <v>260</v>
-      </c>
-      <c r="C117" t="s">
-        <v>260</v>
-      </c>
-      <c r="E117" t="s">
-        <v>27</v>
-      </c>
-      <c r="F117" s="5" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -3878,16 +3908,16 @@
         <v>20</v>
       </c>
       <c r="B118" t="s">
+        <v>261</v>
+      </c>
+      <c r="C118" t="s">
+        <v>261</v>
+      </c>
+      <c r="E118" t="s">
+        <v>26</v>
+      </c>
+      <c r="F118" s="5" t="s">
         <v>262</v>
-      </c>
-      <c r="C118" t="s">
-        <v>262</v>
-      </c>
-      <c r="E118" t="s">
-        <v>27</v>
-      </c>
-      <c r="F118" s="5" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -3895,16 +3925,16 @@
         <v>20</v>
       </c>
       <c r="B119" t="s">
+        <v>263</v>
+      </c>
+      <c r="C119" t="s">
+        <v>263</v>
+      </c>
+      <c r="E119" t="s">
+        <v>26</v>
+      </c>
+      <c r="F119" s="5" t="s">
         <v>264</v>
-      </c>
-      <c r="C119" t="s">
-        <v>264</v>
-      </c>
-      <c r="E119" t="s">
-        <v>27</v>
-      </c>
-      <c r="F119" s="5" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -3912,16 +3942,16 @@
         <v>20</v>
       </c>
       <c r="B120" t="s">
+        <v>265</v>
+      </c>
+      <c r="C120" t="s">
+        <v>265</v>
+      </c>
+      <c r="E120" t="s">
+        <v>26</v>
+      </c>
+      <c r="F120" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="C120" t="s">
-        <v>266</v>
-      </c>
-      <c r="E120" t="s">
-        <v>27</v>
-      </c>
-      <c r="F120" s="5" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -3929,16 +3959,16 @@
         <v>20</v>
       </c>
       <c r="B121" t="s">
+        <v>267</v>
+      </c>
+      <c r="C121" t="s">
+        <v>267</v>
+      </c>
+      <c r="E121" t="s">
+        <v>26</v>
+      </c>
+      <c r="F121" s="5" t="s">
         <v>268</v>
-      </c>
-      <c r="C121" t="s">
-        <v>268</v>
-      </c>
-      <c r="E121" t="s">
-        <v>27</v>
-      </c>
-      <c r="F121" s="5" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -3946,16 +3976,16 @@
         <v>20</v>
       </c>
       <c r="B122" t="s">
+        <v>269</v>
+      </c>
+      <c r="C122" t="s">
+        <v>269</v>
+      </c>
+      <c r="E122" t="s">
+        <v>26</v>
+      </c>
+      <c r="F122" s="5" t="s">
         <v>270</v>
-      </c>
-      <c r="C122" t="s">
-        <v>270</v>
-      </c>
-      <c r="E122" t="s">
-        <v>27</v>
-      </c>
-      <c r="F122" s="5" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -3963,16 +3993,16 @@
         <v>20</v>
       </c>
       <c r="B123" t="s">
+        <v>271</v>
+      </c>
+      <c r="C123" t="s">
+        <v>271</v>
+      </c>
+      <c r="E123" t="s">
+        <v>26</v>
+      </c>
+      <c r="F123" s="5" t="s">
         <v>272</v>
-      </c>
-      <c r="C123" t="s">
-        <v>272</v>
-      </c>
-      <c r="E123" t="s">
-        <v>27</v>
-      </c>
-      <c r="F123" s="5" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -3980,16 +4010,16 @@
         <v>20</v>
       </c>
       <c r="B124" t="s">
+        <v>273</v>
+      </c>
+      <c r="C124" t="s">
+        <v>273</v>
+      </c>
+      <c r="E124" t="s">
+        <v>26</v>
+      </c>
+      <c r="F124" s="5" t="s">
         <v>274</v>
-      </c>
-      <c r="C124" t="s">
-        <v>274</v>
-      </c>
-      <c r="E124" t="s">
-        <v>27</v>
-      </c>
-      <c r="F124" s="5" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -3997,16 +4027,16 @@
         <v>20</v>
       </c>
       <c r="B125" t="s">
+        <v>275</v>
+      </c>
+      <c r="C125" t="s">
+        <v>275</v>
+      </c>
+      <c r="E125" t="s">
+        <v>26</v>
+      </c>
+      <c r="F125" s="5" t="s">
         <v>276</v>
-      </c>
-      <c r="C125" t="s">
-        <v>276</v>
-      </c>
-      <c r="E125" t="s">
-        <v>27</v>
-      </c>
-      <c r="F125" s="5" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -4014,16 +4044,16 @@
         <v>20</v>
       </c>
       <c r="B126" t="s">
+        <v>277</v>
+      </c>
+      <c r="C126" t="s">
+        <v>277</v>
+      </c>
+      <c r="E126" t="s">
+        <v>26</v>
+      </c>
+      <c r="F126" s="5" t="s">
         <v>278</v>
-      </c>
-      <c r="C126" t="s">
-        <v>278</v>
-      </c>
-      <c r="E126" t="s">
-        <v>27</v>
-      </c>
-      <c r="F126" s="5" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -4031,16 +4061,16 @@
         <v>20</v>
       </c>
       <c r="B127" t="s">
+        <v>279</v>
+      </c>
+      <c r="C127" t="s">
+        <v>279</v>
+      </c>
+      <c r="E127" t="s">
+        <v>26</v>
+      </c>
+      <c r="F127" s="5" t="s">
         <v>280</v>
-      </c>
-      <c r="C127" t="s">
-        <v>280</v>
-      </c>
-      <c r="E127" t="s">
-        <v>27</v>
-      </c>
-      <c r="F127" s="5" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -4048,16 +4078,16 @@
         <v>20</v>
       </c>
       <c r="B128" t="s">
+        <v>281</v>
+      </c>
+      <c r="C128" t="s">
+        <v>281</v>
+      </c>
+      <c r="E128" t="s">
+        <v>26</v>
+      </c>
+      <c r="F128" s="5" t="s">
         <v>282</v>
-      </c>
-      <c r="C128" t="s">
-        <v>282</v>
-      </c>
-      <c r="E128" t="s">
-        <v>27</v>
-      </c>
-      <c r="F128" s="5" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -4065,16 +4095,16 @@
         <v>20</v>
       </c>
       <c r="B129" t="s">
+        <v>283</v>
+      </c>
+      <c r="C129" t="s">
+        <v>283</v>
+      </c>
+      <c r="E129" t="s">
+        <v>26</v>
+      </c>
+      <c r="F129" s="5" t="s">
         <v>284</v>
-      </c>
-      <c r="C129" t="s">
-        <v>284</v>
-      </c>
-      <c r="E129" t="s">
-        <v>27</v>
-      </c>
-      <c r="F129" s="5" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
@@ -4082,16 +4112,16 @@
         <v>20</v>
       </c>
       <c r="B130" t="s">
+        <v>285</v>
+      </c>
+      <c r="C130" t="s">
+        <v>285</v>
+      </c>
+      <c r="E130" t="s">
+        <v>26</v>
+      </c>
+      <c r="F130" s="5" t="s">
         <v>286</v>
-      </c>
-      <c r="C130" t="s">
-        <v>286</v>
-      </c>
-      <c r="E130" t="s">
-        <v>27</v>
-      </c>
-      <c r="F130" s="5" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
@@ -4099,16 +4129,16 @@
         <v>20</v>
       </c>
       <c r="B131" t="s">
+        <v>287</v>
+      </c>
+      <c r="C131" t="s">
+        <v>287</v>
+      </c>
+      <c r="E131" t="s">
+        <v>26</v>
+      </c>
+      <c r="F131" s="5" t="s">
         <v>288</v>
-      </c>
-      <c r="C131" t="s">
-        <v>288</v>
-      </c>
-      <c r="E131" t="s">
-        <v>27</v>
-      </c>
-      <c r="F131" s="5" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -4116,16 +4146,16 @@
         <v>20</v>
       </c>
       <c r="B132" t="s">
+        <v>289</v>
+      </c>
+      <c r="C132" t="s">
+        <v>289</v>
+      </c>
+      <c r="E132" t="s">
+        <v>26</v>
+      </c>
+      <c r="F132" s="5" t="s">
         <v>290</v>
-      </c>
-      <c r="C132" t="s">
-        <v>290</v>
-      </c>
-      <c r="E132" t="s">
-        <v>27</v>
-      </c>
-      <c r="F132" s="5" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
@@ -4133,16 +4163,16 @@
         <v>20</v>
       </c>
       <c r="B133" t="s">
+        <v>291</v>
+      </c>
+      <c r="C133" t="s">
+        <v>291</v>
+      </c>
+      <c r="E133" t="s">
+        <v>26</v>
+      </c>
+      <c r="F133" s="5" t="s">
         <v>292</v>
-      </c>
-      <c r="C133" t="s">
-        <v>292</v>
-      </c>
-      <c r="E133" t="s">
-        <v>27</v>
-      </c>
-      <c r="F133" s="5" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
@@ -4150,16 +4180,16 @@
         <v>20</v>
       </c>
       <c r="B134" t="s">
+        <v>293</v>
+      </c>
+      <c r="C134" t="s">
+        <v>293</v>
+      </c>
+      <c r="E134" t="s">
+        <v>26</v>
+      </c>
+      <c r="F134" s="5" t="s">
         <v>294</v>
-      </c>
-      <c r="C134" t="s">
-        <v>294</v>
-      </c>
-      <c r="E134" t="s">
-        <v>27</v>
-      </c>
-      <c r="F134" s="5" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
@@ -4167,16 +4197,16 @@
         <v>20</v>
       </c>
       <c r="B135" t="s">
+        <v>295</v>
+      </c>
+      <c r="C135" t="s">
+        <v>295</v>
+      </c>
+      <c r="E135" t="s">
+        <v>26</v>
+      </c>
+      <c r="F135" s="5" t="s">
         <v>296</v>
-      </c>
-      <c r="C135" t="s">
-        <v>296</v>
-      </c>
-      <c r="E135" t="s">
-        <v>27</v>
-      </c>
-      <c r="F135" s="5" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
@@ -4184,16 +4214,16 @@
         <v>20</v>
       </c>
       <c r="B136" t="s">
+        <v>297</v>
+      </c>
+      <c r="C136" t="s">
+        <v>297</v>
+      </c>
+      <c r="E136" t="s">
+        <v>26</v>
+      </c>
+      <c r="F136" s="5" t="s">
         <v>298</v>
-      </c>
-      <c r="C136" t="s">
-        <v>298</v>
-      </c>
-      <c r="E136" t="s">
-        <v>27</v>
-      </c>
-      <c r="F136" s="5" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
@@ -4201,16 +4231,16 @@
         <v>20</v>
       </c>
       <c r="B137" t="s">
+        <v>299</v>
+      </c>
+      <c r="C137" t="s">
+        <v>299</v>
+      </c>
+      <c r="E137" t="s">
+        <v>26</v>
+      </c>
+      <c r="F137" s="5" t="s">
         <v>300</v>
-      </c>
-      <c r="C137" t="s">
-        <v>300</v>
-      </c>
-      <c r="E137" t="s">
-        <v>27</v>
-      </c>
-      <c r="F137" s="5" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -4218,16 +4248,16 @@
         <v>20</v>
       </c>
       <c r="B138" t="s">
+        <v>301</v>
+      </c>
+      <c r="C138" t="s">
+        <v>301</v>
+      </c>
+      <c r="E138" t="s">
+        <v>26</v>
+      </c>
+      <c r="F138" s="5" t="s">
         <v>302</v>
-      </c>
-      <c r="C138" t="s">
-        <v>302</v>
-      </c>
-      <c r="E138" t="s">
-        <v>27</v>
-      </c>
-      <c r="F138" s="5" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
@@ -4235,16 +4265,16 @@
         <v>20</v>
       </c>
       <c r="B139" t="s">
+        <v>303</v>
+      </c>
+      <c r="C139" t="s">
+        <v>303</v>
+      </c>
+      <c r="E139" t="s">
+        <v>26</v>
+      </c>
+      <c r="F139" s="5" t="s">
         <v>304</v>
-      </c>
-      <c r="C139" t="s">
-        <v>304</v>
-      </c>
-      <c r="E139" t="s">
-        <v>27</v>
-      </c>
-      <c r="F139" s="5" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
@@ -4252,16 +4282,16 @@
         <v>20</v>
       </c>
       <c r="B140" t="s">
+        <v>305</v>
+      </c>
+      <c r="C140" t="s">
+        <v>305</v>
+      </c>
+      <c r="E140" t="s">
+        <v>26</v>
+      </c>
+      <c r="F140" s="5" t="s">
         <v>306</v>
-      </c>
-      <c r="C140" t="s">
-        <v>306</v>
-      </c>
-      <c r="E140" t="s">
-        <v>27</v>
-      </c>
-      <c r="F140" s="5" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
@@ -4269,16 +4299,16 @@
         <v>20</v>
       </c>
       <c r="B141" t="s">
+        <v>307</v>
+      </c>
+      <c r="C141" t="s">
+        <v>307</v>
+      </c>
+      <c r="E141" t="s">
+        <v>26</v>
+      </c>
+      <c r="F141" s="5" t="s">
         <v>308</v>
-      </c>
-      <c r="C141" t="s">
-        <v>308</v>
-      </c>
-      <c r="E141" t="s">
-        <v>27</v>
-      </c>
-      <c r="F141" s="5" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
@@ -4286,16 +4316,16 @@
         <v>20</v>
       </c>
       <c r="B142" t="s">
+        <v>309</v>
+      </c>
+      <c r="C142" t="s">
+        <v>309</v>
+      </c>
+      <c r="E142" t="s">
+        <v>26</v>
+      </c>
+      <c r="F142" s="5" t="s">
         <v>310</v>
-      </c>
-      <c r="C142" t="s">
-        <v>310</v>
-      </c>
-      <c r="E142" t="s">
-        <v>27</v>
-      </c>
-      <c r="F142" s="5" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
@@ -4303,16 +4333,16 @@
         <v>20</v>
       </c>
       <c r="B143" t="s">
+        <v>311</v>
+      </c>
+      <c r="C143" t="s">
+        <v>311</v>
+      </c>
+      <c r="E143" t="s">
+        <v>26</v>
+      </c>
+      <c r="F143" s="5" t="s">
         <v>312</v>
-      </c>
-      <c r="C143" t="s">
-        <v>312</v>
-      </c>
-      <c r="E143" t="s">
-        <v>27</v>
-      </c>
-      <c r="F143" s="5" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
@@ -4320,16 +4350,16 @@
         <v>20</v>
       </c>
       <c r="B144" t="s">
+        <v>313</v>
+      </c>
+      <c r="C144" t="s">
+        <v>313</v>
+      </c>
+      <c r="E144" t="s">
+        <v>26</v>
+      </c>
+      <c r="F144" s="5" t="s">
         <v>314</v>
-      </c>
-      <c r="C144" t="s">
-        <v>314</v>
-      </c>
-      <c r="E144" t="s">
-        <v>27</v>
-      </c>
-      <c r="F144" s="5" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
@@ -4337,16 +4367,16 @@
         <v>20</v>
       </c>
       <c r="B145" t="s">
+        <v>315</v>
+      </c>
+      <c r="C145" t="s">
+        <v>315</v>
+      </c>
+      <c r="E145" t="s">
+        <v>26</v>
+      </c>
+      <c r="F145" s="5" t="s">
         <v>316</v>
-      </c>
-      <c r="C145" t="s">
-        <v>316</v>
-      </c>
-      <c r="E145" t="s">
-        <v>27</v>
-      </c>
-      <c r="F145" s="5" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
@@ -4354,16 +4384,16 @@
         <v>20</v>
       </c>
       <c r="B146" t="s">
+        <v>317</v>
+      </c>
+      <c r="C146" t="s">
+        <v>317</v>
+      </c>
+      <c r="E146" t="s">
+        <v>26</v>
+      </c>
+      <c r="F146" s="5" t="s">
         <v>318</v>
-      </c>
-      <c r="C146" t="s">
-        <v>318</v>
-      </c>
-      <c r="E146" t="s">
-        <v>27</v>
-      </c>
-      <c r="F146" s="5" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
@@ -4371,16 +4401,16 @@
         <v>20</v>
       </c>
       <c r="B147" t="s">
+        <v>319</v>
+      </c>
+      <c r="C147" t="s">
+        <v>319</v>
+      </c>
+      <c r="E147" t="s">
+        <v>26</v>
+      </c>
+      <c r="F147" s="5" t="s">
         <v>320</v>
-      </c>
-      <c r="C147" t="s">
-        <v>320</v>
-      </c>
-      <c r="E147" t="s">
-        <v>27</v>
-      </c>
-      <c r="F147" s="5" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
@@ -4388,16 +4418,16 @@
         <v>20</v>
       </c>
       <c r="B148" t="s">
+        <v>321</v>
+      </c>
+      <c r="C148" t="s">
+        <v>321</v>
+      </c>
+      <c r="E148" t="s">
+        <v>26</v>
+      </c>
+      <c r="F148" s="5" t="s">
         <v>322</v>
-      </c>
-      <c r="C148" t="s">
-        <v>322</v>
-      </c>
-      <c r="E148" t="s">
-        <v>27</v>
-      </c>
-      <c r="F148" s="5" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
@@ -4405,16 +4435,16 @@
         <v>20</v>
       </c>
       <c r="B149" t="s">
+        <v>323</v>
+      </c>
+      <c r="C149" t="s">
+        <v>323</v>
+      </c>
+      <c r="E149" t="s">
+        <v>26</v>
+      </c>
+      <c r="F149" s="5" t="s">
         <v>324</v>
-      </c>
-      <c r="C149" t="s">
-        <v>324</v>
-      </c>
-      <c r="E149" t="s">
-        <v>27</v>
-      </c>
-      <c r="F149" s="5" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
@@ -4422,16 +4452,16 @@
         <v>20</v>
       </c>
       <c r="B150" t="s">
+        <v>325</v>
+      </c>
+      <c r="C150" t="s">
+        <v>325</v>
+      </c>
+      <c r="E150" t="s">
+        <v>26</v>
+      </c>
+      <c r="F150" s="5" t="s">
         <v>326</v>
-      </c>
-      <c r="C150" t="s">
-        <v>326</v>
-      </c>
-      <c r="E150" t="s">
-        <v>27</v>
-      </c>
-      <c r="F150" s="5" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -4439,16 +4469,16 @@
         <v>20</v>
       </c>
       <c r="B151" t="s">
+        <v>327</v>
+      </c>
+      <c r="C151" t="s">
+        <v>327</v>
+      </c>
+      <c r="E151" t="s">
+        <v>26</v>
+      </c>
+      <c r="F151" s="5" t="s">
         <v>328</v>
-      </c>
-      <c r="C151" t="s">
-        <v>328</v>
-      </c>
-      <c r="E151" t="s">
-        <v>27</v>
-      </c>
-      <c r="F151" s="5" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -4456,16 +4486,16 @@
         <v>20</v>
       </c>
       <c r="B152" t="s">
+        <v>329</v>
+      </c>
+      <c r="C152" t="s">
+        <v>329</v>
+      </c>
+      <c r="E152" t="s">
+        <v>26</v>
+      </c>
+      <c r="F152" s="5" t="s">
         <v>330</v>
-      </c>
-      <c r="C152" t="s">
-        <v>330</v>
-      </c>
-      <c r="E152" t="s">
-        <v>27</v>
-      </c>
-      <c r="F152" s="5" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -4473,16 +4503,16 @@
         <v>20</v>
       </c>
       <c r="B153" t="s">
+        <v>331</v>
+      </c>
+      <c r="C153" t="s">
+        <v>331</v>
+      </c>
+      <c r="E153" t="s">
+        <v>26</v>
+      </c>
+      <c r="F153" s="5" t="s">
         <v>332</v>
-      </c>
-      <c r="C153" t="s">
-        <v>332</v>
-      </c>
-      <c r="E153" t="s">
-        <v>27</v>
-      </c>
-      <c r="F153" s="5" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -4490,16 +4520,16 @@
         <v>20</v>
       </c>
       <c r="B154" t="s">
+        <v>333</v>
+      </c>
+      <c r="C154" t="s">
+        <v>333</v>
+      </c>
+      <c r="E154" t="s">
+        <v>26</v>
+      </c>
+      <c r="F154" s="5" t="s">
         <v>334</v>
-      </c>
-      <c r="C154" t="s">
-        <v>334</v>
-      </c>
-      <c r="E154" t="s">
-        <v>27</v>
-      </c>
-      <c r="F154" s="5" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -4507,16 +4537,16 @@
         <v>20</v>
       </c>
       <c r="B155" t="s">
+        <v>335</v>
+      </c>
+      <c r="C155" t="s">
+        <v>335</v>
+      </c>
+      <c r="E155" t="s">
+        <v>26</v>
+      </c>
+      <c r="F155" s="5" t="s">
         <v>336</v>
-      </c>
-      <c r="C155" t="s">
-        <v>336</v>
-      </c>
-      <c r="E155" t="s">
-        <v>27</v>
-      </c>
-      <c r="F155" s="5" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -4524,16 +4554,16 @@
         <v>20</v>
       </c>
       <c r="B156" t="s">
+        <v>337</v>
+      </c>
+      <c r="C156" t="s">
+        <v>337</v>
+      </c>
+      <c r="E156" t="s">
+        <v>26</v>
+      </c>
+      <c r="F156" s="5" t="s">
         <v>338</v>
-      </c>
-      <c r="C156" t="s">
-        <v>338</v>
-      </c>
-      <c r="E156" t="s">
-        <v>27</v>
-      </c>
-      <c r="F156" s="5" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="157" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4541,16 +4571,16 @@
         <v>20</v>
       </c>
       <c r="B157" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C157" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E157" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F157" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -4558,16 +4588,16 @@
         <v>20</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E158" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F158" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -4575,16 +4605,16 @@
         <v>20</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E159" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F159" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -4592,16 +4622,16 @@
         <v>20</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E160" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F160" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -4609,16 +4639,16 @@
         <v>20</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E161" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F161" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -4626,16 +4656,16 @@
         <v>20</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E162" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F162" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -4643,16 +4673,16 @@
         <v>20</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E163" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F163" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -4660,16 +4690,16 @@
         <v>20</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E164" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F164" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -4677,16 +4707,16 @@
         <v>20</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E165" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F165" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -4694,16 +4724,16 @@
         <v>20</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E166" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F166" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -4711,16 +4741,16 @@
         <v>20</v>
       </c>
       <c r="B167" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E167" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F167" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
@@ -4728,16 +4758,16 @@
         <v>20</v>
       </c>
       <c r="B168" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E168" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F168" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -4745,16 +4775,16 @@
         <v>20</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E169" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F169" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -4762,16 +4792,16 @@
         <v>20</v>
       </c>
       <c r="B170" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E170" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F170" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -4779,16 +4809,16 @@
         <v>20</v>
       </c>
       <c r="B171" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E171" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F171" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -4796,16 +4826,16 @@
         <v>20</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E172" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F172" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -4819,7 +4849,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>